<commit_message>
Excel Datos Covid19 Cantabria 200616
</commit_message>
<xml_diff>
--- a/cantabria/2020_covid19_historico.xlsx
+++ b/cantabria/2020_covid19_historico.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abrahamdelgadodiego/Desktop/Dataset Coronavirus/Web SCS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4276E15-DF68-9142-B92C-DA3493E78C29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA09BD66-525D-0947-BB97-BF337FE5525B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="5340" windowWidth="37680" windowHeight="20940" xr2:uid="{300FFF3F-DE0F-9A4B-8B62-5A1F68576C66}"/>
   </bookViews>
@@ -600,11 +600,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3E0C131-480F-424C-B034-FF727A20B2B7}">
-  <dimension ref="A1:AC110"/>
+  <dimension ref="A1:AC111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A110" sqref="A110"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8757,7 +8757,7 @@
         <v>2617</v>
       </c>
       <c r="V102" s="1">
-        <f t="shared" ref="V102:V109" si="3">B102-SUM(T102:U102)</f>
+        <f t="shared" ref="V102:V110" si="3">B102-SUM(T102:U102)</f>
         <v>61</v>
       </c>
       <c r="W102" s="17">
@@ -9351,62 +9351,146 @@
       <c r="W109" s="17">
         <v>76726</v>
       </c>
-      <c r="X109" s="15">
-        <v>13199</v>
-      </c>
+      <c r="X109" s="15"/>
       <c r="Y109" s="17">
         <v>52503</v>
       </c>
-      <c r="Z109" s="15">
-        <v>9032</v>
-      </c>
+      <c r="Z109" s="15"/>
       <c r="AA109" s="17">
         <v>24223</v>
       </c>
-      <c r="AB109" s="15">
-        <v>4167</v>
-      </c>
+      <c r="AB109" s="15"/>
       <c r="AC109" s="15">
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="1:29" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="27" t="s">
+    <row r="110" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A110" s="16">
+        <v>43998</v>
+      </c>
+      <c r="B110" s="17">
+        <v>2923</v>
+      </c>
+      <c r="C110" s="17">
+        <v>2</v>
+      </c>
+      <c r="D110" s="14">
+        <v>0.09</v>
+      </c>
+      <c r="E110" s="17">
+        <v>0.08</v>
+      </c>
+      <c r="F110" s="17">
+        <v>761</v>
+      </c>
+      <c r="G110" s="17">
+        <v>9</v>
+      </c>
+      <c r="H110" s="17">
+        <v>452</v>
+      </c>
+      <c r="I110" s="17">
+        <v>2</v>
+      </c>
+      <c r="J110" s="31">
+        <v>40</v>
+      </c>
+      <c r="K110" s="17">
+        <v>6</v>
+      </c>
+      <c r="L110" s="17">
+        <v>4</v>
+      </c>
+      <c r="M110" s="17">
+        <v>0</v>
+      </c>
+      <c r="N110" s="17">
+        <v>0</v>
+      </c>
+      <c r="O110" s="17">
+        <v>0</v>
+      </c>
+      <c r="P110" s="17">
+        <v>2</v>
+      </c>
+      <c r="Q110" s="17">
+        <v>0</v>
+      </c>
+      <c r="R110" s="17">
+        <v>0</v>
+      </c>
+      <c r="S110" s="17">
+        <v>0</v>
+      </c>
+      <c r="T110" s="17">
+        <v>209</v>
+      </c>
+      <c r="U110" s="17">
+        <v>2668</v>
+      </c>
+      <c r="V110" s="1">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="W110" s="17">
+        <v>77584</v>
+      </c>
+      <c r="X110" s="15">
+        <v>13347</v>
+      </c>
+      <c r="Y110" s="17">
+        <v>53320</v>
+      </c>
+      <c r="Z110" s="15">
+        <v>9173</v>
+      </c>
+      <c r="AA110" s="17">
+        <v>24264</v>
+      </c>
+      <c r="AB110" s="15">
+        <v>4174</v>
+      </c>
+      <c r="AC110" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:29" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B110" s="28"/>
-      <c r="C110" s="28"/>
-      <c r="D110" s="29"/>
-      <c r="E110" s="29"/>
-      <c r="F110" s="28"/>
-      <c r="G110" s="28"/>
-      <c r="H110" s="28"/>
-      <c r="I110" s="28"/>
-      <c r="J110" s="28"/>
-      <c r="K110" s="28"/>
-      <c r="L110" s="28"/>
-      <c r="M110" s="28"/>
-      <c r="N110" s="28"/>
-      <c r="O110" s="28"/>
-      <c r="P110" s="28"/>
-      <c r="Q110" s="28"/>
-      <c r="R110" s="28"/>
-      <c r="S110" s="28"/>
-      <c r="T110" s="28"/>
-      <c r="U110" s="28"/>
-      <c r="V110" s="32"/>
-      <c r="W110" s="28"/>
-      <c r="X110" s="28"/>
-      <c r="Y110" s="30"/>
-      <c r="Z110" s="30"/>
-      <c r="AA110" s="30"/>
-      <c r="AB110" s="30"/>
-      <c r="AC110" s="30"/>
+      <c r="B111" s="28"/>
+      <c r="C111" s="28"/>
+      <c r="D111" s="29"/>
+      <c r="E111" s="29"/>
+      <c r="F111" s="28"/>
+      <c r="G111" s="28"/>
+      <c r="H111" s="28"/>
+      <c r="I111" s="28"/>
+      <c r="J111" s="28"/>
+      <c r="K111" s="28"/>
+      <c r="L111" s="28"/>
+      <c r="M111" s="28"/>
+      <c r="N111" s="28"/>
+      <c r="O111" s="28"/>
+      <c r="P111" s="28"/>
+      <c r="Q111" s="28"/>
+      <c r="R111" s="28"/>
+      <c r="S111" s="28"/>
+      <c r="T111" s="28"/>
+      <c r="U111" s="28"/>
+      <c r="V111" s="32"/>
+      <c r="W111" s="28"/>
+      <c r="X111" s="28"/>
+      <c r="Y111" s="30"/>
+      <c r="Z111" s="30"/>
+      <c r="AA111" s="30"/>
+      <c r="AB111" s="30"/>
+      <c r="AC111" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="V2:V94 V96:V98 V100:V102 V104:V109" formulaRange="1"/>
+    <ignoredError sqref="V2:V94 V96:V98 V100:V102 V104:V110" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>